<commit_message>
Make a waypoint object type.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/levels/Debug.xlsx
+++ b/Assets/StreamingAssets/levels/Debug.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\GameJam_AMDYES\Assets\StreamingAssets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA9B22B-6573-44C5-B754-3827F13D85BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5126231E-FCCD-4034-8DF5-7715E101620F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{C2226A68-D7B0-4D43-ABB2-DEB1751B0BE9}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15"/>
@@ -456,6 +456,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:10">
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
     <row r="4" spans="1:10">
       <c r="C4">
         <v>2</v>

</xml_diff>

<commit_message>
Fix retrieve soul bug.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/levels/Debug.xlsx
+++ b/Assets/StreamingAssets/levels/Debug.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\GameJam_AMDYES\Assets\StreamingAssets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5126231E-FCCD-4034-8DF5-7715E101620F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFD501-D1C7-4E1C-983F-B4236724FD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{C2226A68-D7B0-4D43-ABB2-DEB1751B0BE9}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15"/>
@@ -473,6 +473,9 @@
       </c>
     </row>
     <row r="6" spans="1:10">
+      <c r="A6">
+        <v>6</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>

</xml_diff>